<commit_message>
Corrected error in Codebook_template and added so far untracked file
</commit_message>
<xml_diff>
--- a/data/Codebook_template.xlsx
+++ b/data/Codebook_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://w1maccs.sharepoint.com/sites/SLRforABM/Freigegebene Dokumente/General/Analysis/R-code_git_project/SLR_ABMs_Ecology/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://w1maccs.sharepoint.com/sites/SLRforABM/Freigegebene Dokumente/General/2_Analysis/R-code_git_project/SLR_ABMs_Ecology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{588FB3E4-BBC5-4EDF-85C4-9F46F69E5C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{588FB3E4-BBC5-4EDF-85C4-9F46F69E5C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FF6F6C6-EA58-4710-B8D3-DC0244470D45}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -912,12 +912,6 @@
     <t>Yes/No</t>
   </si>
   <si>
-    <t>Yes/No/Not as questions, but explicit aim or objective</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes/No/No keyword search </t>
-  </si>
-  <si>
     <t>Yes/No/No keyword search applied</t>
   </si>
   <si>
@@ -934,17 +928,30 @@
   </si>
   <si>
     <t>Integer/“N/A”/"No restiction"</t>
+  </si>
+  <si>
+    <t>Yes/No/Not as questions, but explicit aim or obejective</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes/No/No research question </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1445,12 +1452,12 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1462,32 +1469,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -1498,7 +1505,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
@@ -1511,24 +1518,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1536,31 +1543,31 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
@@ -1573,11 +1580,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1587,80 +1594,80 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1669,36 +1676,36 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1710,46 +1717,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2119,17 +2129,17 @@
       <c r="J6" s="2"/>
     </row>
     <row r="10" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="116" t="s">
+      <c r="B10" s="117" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="117"/>
-      <c r="D10" s="117"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="117"/>
-      <c r="G10" s="117"/>
-      <c r="H10" s="117"/>
-      <c r="I10" s="117"/>
-      <c r="J10" s="118"/>
+      <c r="C10" s="118"/>
+      <c r="D10" s="118"/>
+      <c r="E10" s="118"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="118"/>
+      <c r="H10" s="118"/>
+      <c r="I10" s="118"/>
+      <c r="J10" s="119"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -3313,9 +3323,9 @@
   </sheetPr>
   <dimension ref="B1:N1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="6" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I60" sqref="I60"/>
+      <selection pane="topRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -3344,34 +3354,34 @@
       <c r="F2" s="112" t="s">
         <v>192</v>
       </c>
-      <c r="H2" s="125" t="s">
+      <c r="H2" s="126" t="s">
         <v>159</v>
       </c>
-      <c r="I2" s="125"/>
-      <c r="J2" s="125"/>
-      <c r="L2" s="121" t="s">
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="L2" s="122" t="s">
         <v>155</v>
       </c>
-      <c r="M2" s="122"/>
+      <c r="M2" s="123"/>
     </row>
     <row r="3" spans="2:14" ht="14.4" x14ac:dyDescent="0.3">
       <c r="C3" s="6"/>
       <c r="F3" s="7"/>
-      <c r="H3" s="125"/>
-      <c r="I3" s="125"/>
-      <c r="J3" s="125"/>
-      <c r="L3" s="121" t="s">
+      <c r="H3" s="126"/>
+      <c r="I3" s="126"/>
+      <c r="J3" s="126"/>
+      <c r="L3" s="122" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="122"/>
+      <c r="M3" s="123"/>
     </row>
     <row r="4" spans="2:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="6"/>
       <c r="F4" s="7"/>
-      <c r="L4" s="123" t="s">
+      <c r="L4" s="124" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="124"/>
+      <c r="M4" s="125"/>
     </row>
     <row r="5" spans="2:14" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="8" t="s">
@@ -3471,8 +3481,8 @@
       <c r="G9" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="114" t="s">
-        <v>194</v>
+      <c r="H9" s="115" t="s">
+        <v>200</v>
       </c>
       <c r="I9" s="76" t="s">
         <v>140</v>
@@ -3500,8 +3510,8 @@
       <c r="G10" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="32" t="s">
-        <v>195</v>
+      <c r="H10" s="116" t="s">
+        <v>201</v>
       </c>
       <c r="I10" s="79" t="s">
         <v>141</v>
@@ -3702,7 +3712,7 @@
         <v>33</v>
       </c>
       <c r="H20" s="26" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I20" s="54" t="s">
         <v>52</v>
@@ -3731,7 +3741,7 @@
         <v>33</v>
       </c>
       <c r="H21" s="26" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I21" s="54" t="s">
         <v>183</v>
@@ -3758,7 +3768,7 @@
         <v>33</v>
       </c>
       <c r="H22" s="36" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="I22" s="37" t="s">
         <v>182</v>
@@ -3888,7 +3898,7 @@
         <v>33</v>
       </c>
       <c r="H27" s="26" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I27" s="54"/>
       <c r="J27" s="24" t="s">
@@ -4413,7 +4423,7 @@
       </c>
       <c r="G48" s="29"/>
       <c r="H48" s="86" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I48" s="33" t="s">
         <v>80</v>
@@ -4469,7 +4479,7 @@
         <v>33</v>
       </c>
       <c r="H50" s="100" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I50" s="37" t="s">
         <v>175</v>
@@ -4716,8 +4726,8 @@
       <c r="G61" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H61" s="115" t="s">
-        <v>199</v>
+      <c r="H61" s="114" t="s">
+        <v>197</v>
       </c>
       <c r="I61" s="37" t="s">
         <v>86</v>
@@ -4820,7 +4830,7 @@
         <v>33</v>
       </c>
       <c r="H65" s="26" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="I65" s="67"/>
       <c r="J65" s="24" t="s">
@@ -5081,7 +5091,7 @@
       <c r="H77" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="I77" s="119" t="s">
+      <c r="I77" s="120" t="s">
         <v>149</v>
       </c>
       <c r="L77" s="38"/>
@@ -5101,7 +5111,7 @@
       <c r="H78" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="I78" s="120"/>
+      <c r="I78" s="121"/>
       <c r="L78" s="38"/>
       <c r="M78" s="39"/>
     </row>
@@ -5119,7 +5129,7 @@
       <c r="H79" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="I79" s="120"/>
+      <c r="I79" s="121"/>
       <c r="L79" s="38"/>
       <c r="M79" s="39"/>
     </row>
@@ -9329,6 +9339,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dc8ea9bb-7be6-4347-bbbd-43ecd0226ab6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="36965efa-5a39-45c9-9312-a4f852bee1e3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E28E13ACBC000A4C890C7EF62115DE09" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="38c6947b388da27d619d5996577e48bb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="dc8ea9bb-7be6-4347-bbbd-43ecd0226ab6" xmlns:ns3="36965efa-5a39-45c9-9312-a4f852bee1e3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b0d313870efd85b4f0f8b7717aad82c" ns2:_="" ns3:_="">
     <xsd:import namespace="dc8ea9bb-7be6-4347-bbbd-43ecd0226ab6"/>
@@ -9553,27 +9583,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{118A9060-EF27-4670-A7BD-5FE79C142D77}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dc8ea9bb-7be6-4347-bbbd-43ecd0226ab6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="36965efa-5a39-45c9-9312-a4f852bee1e3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072C8801-02D8-41B4-9C3A-C0871C6DF7B0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dc8ea9bb-7be6-4347-bbbd-43ecd0226ab6"/>
+    <ds:schemaRef ds:uri="36965efa-5a39-45c9-9312-a4f852bee1e3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ACD51B1-C9C5-4587-980D-DB52F05C9F9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9590,23 +9619,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{118A9060-EF27-4670-A7BD-5FE79C142D77}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072C8801-02D8-41B4-9C3A-C0871C6DF7B0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dc8ea9bb-7be6-4347-bbbd-43ecd0226ab6"/>
-    <ds:schemaRef ds:uri="36965efa-5a39-45c9-9312-a4f852bee1e3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>